<commit_message>
fixed replit's indentation weirdness, add excel file.
</commit_message>
<xml_diff>
--- a/function timing graph.xlsx
+++ b/function timing graph.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jroach/PycharmProjects/InbornChocolateAssociate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DC9975E6-C112-8347-B6E6-9C0EBACAB81B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B9F75E-EE1B-034C-8C9B-91CA15B8171E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="500" windowWidth="28040" windowHeight="16260"/>
+    <workbookView xWindow="360" yWindow="500" windowWidth="28040" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fib_bad" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>i</t>
   </si>
@@ -55,11 +55,14 @@
   <si>
     <t>log good fib time</t>
   </si>
+  <si>
+    <t>sdfd</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -2482,11 +2485,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" activeCellId="1" sqref="A1:A31 E1:G31"/>
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2913,7 +2916,7 @@
         <v>-5.9329291439546932</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2939,7 +2942,7 @@
         <v>-5.9999999999995657</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
@@ -2965,7 +2968,7 @@
         <v>-5.9329291439546932</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
@@ -2991,7 +2994,7 @@
         <v>-5.5949953349493349</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>18</v>
       </c>
@@ -3017,7 +3020,7 @@
         <v>-5.726998727935829</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>19</v>
       </c>
@@ -3043,7 +3046,7 @@
         <v>-5.6092414712607068</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
@@ -3069,7 +3072,7 @@
         <v>-5.7891466346856015</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>21</v>
       </c>
@@ -3095,7 +3098,7 @@
         <v>-5.2531323721493033</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>22</v>
       </c>
@@ -3121,7 +3124,7 @@
         <v>-5.6813107300522665</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>23</v>
       </c>
@@ -3147,7 +3150,7 @@
         <v>-5.2218487496164245</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>24</v>
       </c>
@@ -3173,7 +3176,7 @@
         <v>-5.8616973018343819</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>25</v>
       </c>
@@ -3199,7 +3202,7 @@
         <v>-5.6020599913275282</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>26</v>
       </c>
@@ -3225,7 +3228,7 @@
         <v>-5.8486301497514512</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>27</v>
       </c>
@@ -3251,7 +3254,7 @@
         <v>-5.6989700043355844</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>28</v>
       </c>
@@ -3277,7 +3280,7 @@
         <v>-5.5228787452799031</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>29</v>
       </c>
@@ -3301,6 +3304,11 @@
       <c r="G31">
         <f t="shared" si="3"/>
         <v>-5.4025242101267583</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I32" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>